<commit_message>
Add stok and penjualan management features
- Created views for exporting PDF and Excel for stok and penjualan.
- Implemented AJAX functionality for managing stok and penjualan, including create, edit, delete, and show modals.
- Enhanced the welcome page with summary cards for total penjualan, total stok, and total pengguna.
- Updated the change password form with required fields and localized labels.
- Removed the delete profile picture modal as it is no longer needed.
- Added DataTables for displaying penjualan and stok data with server-side processing.
- Updated routes for stok and penjualan management.
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/POS/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C422B892-1A12-BE4A-AA65-56C260763AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC954AF-7C50-E340-A2AE-EB9BD70380D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5D49F5CC-1196-F949-9D25-E0F70F6ED8BE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{5D49F5CC-1196-F949-9D25-E0F70F6ED8BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>kategori_id</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Cleo 600ml</t>
+  </si>
+  <si>
+    <t>supplier_id</t>
+  </si>
+  <si>
+    <t>stok</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB7BDC7-4A9E-2248-80F9-7B40F46BACFD}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,7 +459,7 @@
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +475,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,8 +498,14 @@
       <c r="E2">
         <v>25000</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -503,8 +521,14 @@
       <c r="E3">
         <v>12500</v>
       </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -520,8 +544,14 @@
       <c r="E4">
         <v>18500</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -537,8 +567,14 @@
       <c r="E5">
         <v>92500</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -553,6 +589,12 @@
       </c>
       <c r="E6">
         <v>4300</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>